<commit_message>
Replace Progreso sheet with visual Dashboard
- 5 KPI cards: total sessions, last workout, max weight, avg reps, total volume
- Bar chart: sessions per day of the week
- Pie chart: percentage distribution by routine with colored slices
- Line chart: weight progression over time (references Registro directly)
- 6 insight metrics: days since last workout, weekly/monthly sessions,
  most frequent exercise, avg series, max single-entry volume
- Last 10 entries table
- Updated instructions to describe new Dashboard sheet

https://claude.ai/code/session_01VPVYV7Huumm7PzRCnN9SP3
</commit_message>
<xml_diff>
--- a/Entrenamiento_Casa.xlsx
+++ b/Entrenamiento_Casa.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Registro" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Datos" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="Rutinas" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Progreso" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Dashboard" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Instrucciones" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
@@ -28,10 +28,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -76,6 +77,18 @@
       <b val="1"/>
       <color rgb="00FFFFFF"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="22"/>
     </font>
   </fonts>
   <fills count="12">
@@ -162,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -230,9 +243,50 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -307,6 +361,409 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Sesiones por Día</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Dashboard'!C10</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill>
+              <a:srgbClr val="2E5090"/>
+            </a:solidFill>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Dashboard'!$B$11:$B$15</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Dashboard'!$C$11:$C$15</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Sesiones</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Distribución por Rutina</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Dashboard'!C10</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <dPt>
+            <idx val="0"/>
+            <spPr>
+              <a:solidFill>
+                <a:srgbClr val="2E5090"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
+          <dPt>
+            <idx val="1"/>
+            <spPr>
+              <a:solidFill>
+                <a:srgbClr val="27AE60"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
+          <dPt>
+            <idx val="2"/>
+            <spPr>
+              <a:solidFill>
+                <a:srgbClr val="E67E22"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
+          <dPt>
+            <idx val="3"/>
+            <spPr>
+              <a:solidFill>
+                <a:srgbClr val="E74C3C"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
+          <dPt>
+            <idx val="4"/>
+            <spPr>
+              <a:solidFill>
+                <a:srgbClr val="1B2A4A"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
+          <cat>
+            <numRef>
+              <f>'Dashboard'!$B$11:$B$15</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Dashboard'!$C$11:$C$15</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showVal val="0"/>
+          <showCatName val="1"/>
+          <showPercent val="1"/>
+        </dLbls>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Peso Levantado por Sesión</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Registro'!F11</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln w="22000">
+              <a:solidFill>
+                <a:srgbClr val="27AE60"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'Registro'!$F$12:$F$200</f>
+            </numRef>
+          </val>
+          <smooth val="1"/>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Entrada</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Peso (kg)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>8</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7200000" cy="4320000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>21</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7200000" cy="4320000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7200000" cy="4320000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3625,539 +4082,687 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="2" customWidth="1" min="1" max="1"/>
+    <col width="26" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="2" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>RESUMEN DE PROGRESO</t>
+          <t>DASHBOARD DE ENTRENAMIENTO</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
       <c r="C1" s="2" t="n"/>
       <c r="D1" s="2" t="n"/>
       <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="27" t="inlineStr">
         <is>
-          <t>Estadísticas calculadas automáticamente desde tu historial.</t>
+          <t>Resumen visual de tu progreso. Los datos se actualizan automáticamente desde la hoja Registro.</t>
         </is>
       </c>
       <c r="B2" s="28" t="n"/>
       <c r="C2" s="28" t="n"/>
       <c r="D2" s="28" t="n"/>
       <c r="E2" s="28" t="n"/>
+      <c r="F2" s="28" t="n"/>
+      <c r="G2" s="28" t="n"/>
+      <c r="H2" s="28" t="n"/>
+      <c r="I2" s="28" t="n"/>
+      <c r="J2" s="28" t="n"/>
+      <c r="K2" s="28" t="n"/>
+      <c r="L2" s="28" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="5" t="inlineStr">
         <is>
-          <t>ESTADÍSTICAS GENERALES</t>
+          <t>MÉTRICAS CLAVE</t>
         </is>
       </c>
       <c r="B4" s="6" t="n"/>
       <c r="C4" s="6" t="n"/>
       <c r="D4" s="6" t="n"/>
       <c r="E4" s="6" t="n"/>
+      <c r="F4" s="6" t="n"/>
+      <c r="G4" s="6" t="n"/>
+      <c r="H4" s="6" t="n"/>
+      <c r="I4" s="6" t="n"/>
+      <c r="J4" s="6" t="n"/>
+      <c r="K4" s="6" t="n"/>
+      <c r="L4" s="6" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="29" t="inlineStr">
-        <is>
-          <t>Total sesiones registradas</t>
-        </is>
-      </c>
-      <c r="B5" s="9">
+      <c r="B5" s="29" t="inlineStr">
+        <is>
+          <t>Total Sesiones</t>
+        </is>
+      </c>
+      <c r="C5" s="12" t="n"/>
+      <c r="D5" s="30" t="inlineStr">
+        <is>
+          <t>Último Entreno</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="n"/>
+      <c r="F5" s="31" t="inlineStr">
+        <is>
+          <t>Peso Máx (kg)</t>
+        </is>
+      </c>
+      <c r="G5" s="14" t="n"/>
+      <c r="H5" s="32" t="inlineStr">
+        <is>
+          <t>Prom. Reps</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="n"/>
+      <c r="J5" s="33" t="inlineStr">
+        <is>
+          <t>Volumen Total</t>
+        </is>
+      </c>
+      <c r="K5" s="16" t="n"/>
+    </row>
+    <row r="6">
+      <c r="B6" s="34">
         <f>COUNTA(Registro!A12:A200)</f>
         <v/>
       </c>
-      <c r="C5" s="4" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="29" t="inlineStr">
-        <is>
-          <t>Último entrenamiento</t>
-        </is>
-      </c>
-      <c r="B6" s="8">
-        <f>MAX(Registro!A12:A200)</f>
-        <v/>
-      </c>
-      <c r="C6" s="4" t="n"/>
+      <c r="C6" s="12" t="n"/>
+      <c r="D6" s="35">
+        <f>IF(COUNTA(Registro!A12:A200)&gt;0,MAX(Registro!A12:A200),"-")</f>
+        <v/>
+      </c>
+      <c r="E6" s="6" t="n"/>
+      <c r="F6" s="36">
+        <f>IF(MAX(Registro!F12:F200)&gt;0,MAX(Registro!F12:F200),"-")</f>
+        <v/>
+      </c>
+      <c r="G6" s="14" t="n"/>
+      <c r="H6" s="37">
+        <f>IFERROR(ROUND(AVERAGE(Registro!E12:E200),1),"-")</f>
+        <v/>
+      </c>
+      <c r="I6" s="2" t="n"/>
+      <c r="J6" s="38">
+        <f>IFERROR(SUMPRODUCT((Registro!D12:D200)*(Registro!E12:E200)),"-")</f>
+        <v/>
+      </c>
+      <c r="K6" s="16" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="29" t="inlineStr">
-        <is>
-          <t>Peso máximo levantado (kg)</t>
-        </is>
-      </c>
-      <c r="B7" s="9">
-        <f>MAX(Registro!F12:F200)</f>
-        <v/>
-      </c>
-      <c r="C7" s="4" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="29" t="inlineStr">
-        <is>
-          <t>Promedio de repeticiones</t>
-        </is>
-      </c>
-      <c r="B8" s="9">
-        <f>IFERROR(AVERAGE(Registro!E12:E200),"")</f>
-        <v/>
-      </c>
-      <c r="C8" s="4" t="n"/>
+      <c r="B7" s="12" t="n"/>
+      <c r="C7" s="12" t="n"/>
+      <c r="D7" s="6" t="n"/>
+      <c r="E7" s="6" t="n"/>
+      <c r="F7" s="14" t="n"/>
+      <c r="G7" s="14" t="n"/>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
+      <c r="J7" s="16" t="n"/>
+      <c r="K7" s="16" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="29" t="inlineStr">
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>VOLUMEN POR DÍA DE RUTINA</t>
+        </is>
+      </c>
+      <c r="C9" s="6" t="n"/>
+      <c r="D9" s="6" t="n"/>
+      <c r="E9" s="6" t="n"/>
+      <c r="F9" s="6" t="n"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="11" t="inlineStr">
+        <is>
+          <t>Día</t>
+        </is>
+      </c>
+      <c r="C10" s="11" t="inlineStr">
+        <is>
+          <t>Sesiones</t>
+        </is>
+      </c>
+      <c r="D10" s="11" t="inlineStr">
+        <is>
+          <t>Series</t>
+        </is>
+      </c>
+      <c r="E10" s="11" t="inlineStr">
+        <is>
+          <t>Reps</t>
+        </is>
+      </c>
+      <c r="F10" s="11" t="inlineStr">
+        <is>
+          <t>Peso Prom.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="39" t="inlineStr">
+        <is>
+          <t>Lunes</t>
+        </is>
+      </c>
+      <c r="C11" s="20">
+        <f>COUNTIF(Registro!B$12:B$200,"Lunes - Pecho y Tríceps")</f>
+        <v/>
+      </c>
+      <c r="D11" s="20">
+        <f>SUMIF(Registro!B$12:B$200,"Lunes - Pecho y Tríceps",Registro!D$12:D$200)</f>
+        <v/>
+      </c>
+      <c r="E11" s="20">
+        <f>SUMIF(Registro!B$12:B$200,"Lunes - Pecho y Tríceps",Registro!E$12:E$200)</f>
+        <v/>
+      </c>
+      <c r="F11" s="20">
+        <f>IFERROR(AVERAGEIF(Registro!B$12:B$200,"Lunes - Pecho y Tríceps",Registro!F$12:F$200),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="40" t="inlineStr">
+        <is>
+          <t>Martes</t>
+        </is>
+      </c>
+      <c r="C12" s="22">
+        <f>COUNTIF(Registro!B$12:B$200,"Martes - Espalda y Bíceps")</f>
+        <v/>
+      </c>
+      <c r="D12" s="22">
+        <f>SUMIF(Registro!B$12:B$200,"Martes - Espalda y Bíceps",Registro!D$12:D$200)</f>
+        <v/>
+      </c>
+      <c r="E12" s="22">
+        <f>SUMIF(Registro!B$12:B$200,"Martes - Espalda y Bíceps",Registro!E$12:E$200)</f>
+        <v/>
+      </c>
+      <c r="F12" s="22">
+        <f>IFERROR(AVERAGEIF(Registro!B$12:B$200,"Martes - Espalda y Bíceps",Registro!F$12:F$200),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="39" t="inlineStr">
+        <is>
+          <t>Miércoles</t>
+        </is>
+      </c>
+      <c r="C13" s="20">
+        <f>COUNTIF(Registro!B$12:B$200,"Miércoles - Piernas")</f>
+        <v/>
+      </c>
+      <c r="D13" s="20">
+        <f>SUMIF(Registro!B$12:B$200,"Miércoles - Piernas",Registro!D$12:D$200)</f>
+        <v/>
+      </c>
+      <c r="E13" s="20">
+        <f>SUMIF(Registro!B$12:B$200,"Miércoles - Piernas",Registro!E$12:E$200)</f>
+        <v/>
+      </c>
+      <c r="F13" s="20">
+        <f>IFERROR(AVERAGEIF(Registro!B$12:B$200,"Miércoles - Piernas",Registro!F$12:F$200),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="40" t="inlineStr">
+        <is>
+          <t>Jueves</t>
+        </is>
+      </c>
+      <c r="C14" s="22">
+        <f>COUNTIF(Registro!B$12:B$200,"Jueves - Hombros y Core")</f>
+        <v/>
+      </c>
+      <c r="D14" s="22">
+        <f>SUMIF(Registro!B$12:B$200,"Jueves - Hombros y Core",Registro!D$12:D$200)</f>
+        <v/>
+      </c>
+      <c r="E14" s="22">
+        <f>SUMIF(Registro!B$12:B$200,"Jueves - Hombros y Core",Registro!E$12:E$200)</f>
+        <v/>
+      </c>
+      <c r="F14" s="22">
+        <f>IFERROR(AVERAGEIF(Registro!B$12:B$200,"Jueves - Hombros y Core",Registro!F$12:F$200),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="39" t="inlineStr">
+        <is>
+          <t>Viernes</t>
+        </is>
+      </c>
+      <c r="C15" s="20">
+        <f>COUNTIF(Registro!B$12:B$200,"Viernes - Full Body")</f>
+        <v/>
+      </c>
+      <c r="D15" s="20">
+        <f>SUMIF(Registro!B$12:B$200,"Viernes - Full Body",Registro!D$12:D$200)</f>
+        <v/>
+      </c>
+      <c r="E15" s="20">
+        <f>SUMIF(Registro!B$12:B$200,"Viernes - Full Body",Registro!E$12:E$200)</f>
+        <v/>
+      </c>
+      <c r="F15" s="20">
+        <f>IFERROR(AVERAGEIF(Registro!B$12:B$200,"Viernes - Full Body",Registro!F$12:F$200),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="17" t="inlineStr">
+        <is>
+          <t>INSIGHTS</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n"/>
+      <c r="D17" s="2" t="n"/>
+      <c r="E17" s="2" t="n"/>
+      <c r="F17" s="2" t="n"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="39" t="inlineStr">
+        <is>
+          <t>Días sin entrenar</t>
+        </is>
+      </c>
+      <c r="C18" s="41">
+        <f>IF(COUNTA(Registro!A12:A200)&gt;0,TODAY()-MAX(Registro!A12:A200),"-")</f>
+        <v/>
+      </c>
+      <c r="D18" s="42" t="n"/>
+      <c r="E18" s="42" t="n"/>
+      <c r="F18" s="42" t="n"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="40" t="inlineStr">
+        <is>
+          <t>Sesiones esta semana</t>
+        </is>
+      </c>
+      <c r="C19" s="43">
+        <f>COUNTIFS(Registro!A12:A200,"&gt;="&amp;(TODAY()-WEEKDAY(TODAY(),2)+1),Registro!A12:A200,"&lt;="&amp;TODAY())</f>
+        <v/>
+      </c>
+      <c r="D19" s="44" t="n"/>
+      <c r="E19" s="44" t="n"/>
+      <c r="F19" s="44" t="n"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="39" t="inlineStr">
+        <is>
+          <t>Sesiones este mes</t>
+        </is>
+      </c>
+      <c r="C20" s="41">
+        <f>COUNTIFS(Registro!A12:A200,"&gt;="&amp;DATE(YEAR(TODAY()),MONTH(TODAY()),1),Registro!A12:A200,"&lt;="&amp;TODAY())</f>
+        <v/>
+      </c>
+      <c r="D20" s="42" t="n"/>
+      <c r="E20" s="42" t="n"/>
+      <c r="F20" s="42" t="n"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="40" t="inlineStr">
         <is>
           <t>Ejercicio más frecuente</t>
         </is>
       </c>
-      <c r="B9" s="9">
-        <f>IFERROR(INDEX(Registro!C12:C200,MATCH(MAX(COUNTIF(Registro!C12:C200,Registro!C12:C200)),COUNTIF(Registro!C12:C200,Registro!C12:C200),0)),"")</f>
-        <v/>
-      </c>
-      <c r="C9" s="4" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="5" t="inlineStr">
-        <is>
-          <t>VOLUMEN POR DÍA DE RUTINA</t>
-        </is>
-      </c>
-      <c r="B12" s="6" t="n"/>
-      <c r="C12" s="6" t="n"/>
-      <c r="D12" s="6" t="n"/>
-      <c r="E12" s="6" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="11" t="inlineStr">
-        <is>
-          <t>Día / Rutina</t>
-        </is>
-      </c>
-      <c r="B13" s="11" t="inlineStr">
-        <is>
-          <t>Sesiones</t>
-        </is>
-      </c>
-      <c r="C13" s="11" t="inlineStr">
-        <is>
-          <t>Total Series</t>
-        </is>
-      </c>
-      <c r="D13" s="11" t="inlineStr">
-        <is>
-          <t>Total Reps</t>
-        </is>
-      </c>
-      <c r="E13" s="11" t="inlineStr">
-        <is>
-          <t>Peso Prom. (kg)</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="26" t="inlineStr">
-        <is>
-          <t>Lunes - Pecho y Tríceps</t>
-        </is>
-      </c>
-      <c r="B14" s="20">
-        <f>COUNTIF(Registro!B12:B200,A14)</f>
-        <v/>
-      </c>
-      <c r="C14" s="20">
-        <f>SUMIF(Registro!B12:B200,A14,Registro!D12:D200)</f>
-        <v/>
-      </c>
-      <c r="D14" s="20">
-        <f>SUMIF(Registro!B12:B200,A14,Registro!E12:E200)</f>
-        <v/>
-      </c>
-      <c r="E14" s="20">
-        <f>IFERROR(AVERAGEIF(Registro!B12:B200,A14,Registro!F12:F200),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="25" t="inlineStr">
-        <is>
-          <t>Martes - Espalda y Bíceps</t>
-        </is>
-      </c>
-      <c r="B15" s="22">
-        <f>COUNTIF(Registro!B12:B200,A15)</f>
-        <v/>
-      </c>
-      <c r="C15" s="22">
-        <f>SUMIF(Registro!B12:B200,A15,Registro!D12:D200)</f>
-        <v/>
-      </c>
-      <c r="D15" s="22">
-        <f>SUMIF(Registro!B12:B200,A15,Registro!E12:E200)</f>
-        <v/>
-      </c>
-      <c r="E15" s="22">
-        <f>IFERROR(AVERAGEIF(Registro!B12:B200,A15,Registro!F12:F200),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="26" t="inlineStr">
-        <is>
-          <t>Miércoles - Piernas</t>
-        </is>
-      </c>
-      <c r="B16" s="20">
-        <f>COUNTIF(Registro!B12:B200,A16)</f>
-        <v/>
-      </c>
-      <c r="C16" s="20">
-        <f>SUMIF(Registro!B12:B200,A16,Registro!D12:D200)</f>
-        <v/>
-      </c>
-      <c r="D16" s="20">
-        <f>SUMIF(Registro!B12:B200,A16,Registro!E12:E200)</f>
-        <v/>
-      </c>
-      <c r="E16" s="20">
-        <f>IFERROR(AVERAGEIF(Registro!B12:B200,A16,Registro!F12:F200),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="25" t="inlineStr">
-        <is>
-          <t>Jueves - Hombros y Core</t>
-        </is>
-      </c>
-      <c r="B17" s="22">
-        <f>COUNTIF(Registro!B12:B200,A17)</f>
-        <v/>
-      </c>
-      <c r="C17" s="22">
-        <f>SUMIF(Registro!B12:B200,A17,Registro!D12:D200)</f>
-        <v/>
-      </c>
-      <c r="D17" s="22">
-        <f>SUMIF(Registro!B12:B200,A17,Registro!E12:E200)</f>
-        <v/>
-      </c>
-      <c r="E17" s="22">
-        <f>IFERROR(AVERAGEIF(Registro!B12:B200,A17,Registro!F12:F200),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="26" t="inlineStr">
-        <is>
-          <t>Viernes - Full Body</t>
-        </is>
-      </c>
-      <c r="B18" s="20">
-        <f>COUNTIF(Registro!B12:B200,A18)</f>
-        <v/>
-      </c>
-      <c r="C18" s="20">
-        <f>SUMIF(Registro!B12:B200,A18,Registro!D12:D200)</f>
-        <v/>
-      </c>
-      <c r="D18" s="20">
-        <f>SUMIF(Registro!B12:B200,A18,Registro!E12:E200)</f>
-        <v/>
-      </c>
-      <c r="E18" s="20">
-        <f>IFERROR(AVERAGEIF(Registro!B12:B200,A18,Registro!F12:F200),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="inlineStr">
+      <c r="C21" s="43">
+        <f>IFERROR(INDEX(Registro!C12:C200,MATCH(MAX(COUNTIF(Registro!C12:C200,Registro!C12:C200)),COUNTIF(Registro!C12:C200,Registro!C12:C200),0)),"-")</f>
+        <v/>
+      </c>
+      <c r="D21" s="44" t="n"/>
+      <c r="E21" s="44" t="n"/>
+      <c r="F21" s="44" t="n"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="39" t="inlineStr">
+        <is>
+          <t>Prom. series por sesión</t>
+        </is>
+      </c>
+      <c r="C22" s="41">
+        <f>IFERROR(ROUND(AVERAGE(Registro!D12:D200),1),"-")</f>
+        <v/>
+      </c>
+      <c r="D22" s="42" t="n"/>
+      <c r="E22" s="42" t="n"/>
+      <c r="F22" s="42" t="n"/>
+    </row>
+    <row r="23">
+      <c r="B23" s="40" t="inlineStr">
+        <is>
+          <t>Mayor volumen en 1 registro</t>
+        </is>
+      </c>
+      <c r="C23" s="43">
+        <f>IFERROR(MAX(Registro!D12:D200*Registro!E12:E200),"-")</f>
+        <v/>
+      </c>
+      <c r="D23" s="44" t="n"/>
+      <c r="E23" s="44" t="n"/>
+      <c r="F23" s="44" t="n"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="17" t="inlineStr">
         <is>
           <t>ÚLTIMOS 10 REGISTROS</t>
         </is>
       </c>
-      <c r="B21" s="6" t="n"/>
-      <c r="C21" s="6" t="n"/>
-      <c r="D21" s="6" t="n"/>
-      <c r="E21" s="6" t="n"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="11" t="inlineStr">
+      <c r="C26" s="2" t="n"/>
+      <c r="D26" s="2" t="n"/>
+      <c r="E26" s="2" t="n"/>
+      <c r="F26" s="2" t="n"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="11" t="inlineStr">
         <is>
           <t>Fecha</t>
         </is>
       </c>
-      <c r="B22" s="11" t="inlineStr">
+      <c r="C27" s="11" t="inlineStr">
         <is>
           <t>Rutina</t>
         </is>
       </c>
-      <c r="C22" s="11" t="inlineStr">
+      <c r="D27" s="11" t="inlineStr">
         <is>
           <t>Ejercicio</t>
         </is>
       </c>
-      <c r="D22" s="11" t="inlineStr">
+      <c r="E27" s="11" t="inlineStr">
         <is>
           <t>Reps</t>
         </is>
       </c>
-      <c r="E22" s="11" t="inlineStr">
+      <c r="F27" s="11" t="inlineStr">
         <is>
           <t>Peso (kg)</t>
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="19">
+    <row r="28">
+      <c r="B28" s="19">
         <f>IFERROR(INDEX(Registro!A$12:A$200,COUNTA(Registro!A$12:A$200)-0),"")</f>
         <v/>
       </c>
-      <c r="B23" s="20">
+      <c r="C28" s="20">
         <f>IFERROR(INDEX(Registro!B$12:B$200,COUNTA(Registro!A$12:A$200)-0),"")</f>
         <v/>
       </c>
-      <c r="C23" s="20">
+      <c r="D28" s="20">
         <f>IFERROR(INDEX(Registro!C$12:C$200,COUNTA(Registro!A$12:A$200)-0),"")</f>
         <v/>
       </c>
-      <c r="D23" s="20">
+      <c r="E28" s="20">
         <f>IFERROR(INDEX(Registro!E$12:E$200,COUNTA(Registro!A$12:A$200)-0),"")</f>
         <v/>
       </c>
-      <c r="E23" s="20">
+      <c r="F28" s="20">
         <f>IFERROR(INDEX(Registro!F$12:F$200,COUNTA(Registro!A$12:A$200)-0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="21">
+    <row r="29">
+      <c r="B29" s="21">
         <f>IFERROR(INDEX(Registro!A$12:A$200,COUNTA(Registro!A$12:A$200)-1),"")</f>
         <v/>
       </c>
-      <c r="B24" s="22">
+      <c r="C29" s="22">
         <f>IFERROR(INDEX(Registro!B$12:B$200,COUNTA(Registro!A$12:A$200)-1),"")</f>
         <v/>
       </c>
-      <c r="C24" s="22">
+      <c r="D29" s="22">
         <f>IFERROR(INDEX(Registro!C$12:C$200,COUNTA(Registro!A$12:A$200)-1),"")</f>
         <v/>
       </c>
-      <c r="D24" s="22">
+      <c r="E29" s="22">
         <f>IFERROR(INDEX(Registro!E$12:E$200,COUNTA(Registro!A$12:A$200)-1),"")</f>
         <v/>
       </c>
-      <c r="E24" s="22">
+      <c r="F29" s="22">
         <f>IFERROR(INDEX(Registro!F$12:F$200,COUNTA(Registro!A$12:A$200)-1),"")</f>
         <v/>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="19">
+    <row r="30">
+      <c r="B30" s="19">
         <f>IFERROR(INDEX(Registro!A$12:A$200,COUNTA(Registro!A$12:A$200)-2),"")</f>
         <v/>
       </c>
-      <c r="B25" s="20">
+      <c r="C30" s="20">
         <f>IFERROR(INDEX(Registro!B$12:B$200,COUNTA(Registro!A$12:A$200)-2),"")</f>
         <v/>
       </c>
-      <c r="C25" s="20">
+      <c r="D30" s="20">
         <f>IFERROR(INDEX(Registro!C$12:C$200,COUNTA(Registro!A$12:A$200)-2),"")</f>
         <v/>
       </c>
-      <c r="D25" s="20">
+      <c r="E30" s="20">
         <f>IFERROR(INDEX(Registro!E$12:E$200,COUNTA(Registro!A$12:A$200)-2),"")</f>
         <v/>
       </c>
-      <c r="E25" s="20">
+      <c r="F30" s="20">
         <f>IFERROR(INDEX(Registro!F$12:F$200,COUNTA(Registro!A$12:A$200)-2),"")</f>
         <v/>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="21">
+    <row r="31">
+      <c r="B31" s="21">
         <f>IFERROR(INDEX(Registro!A$12:A$200,COUNTA(Registro!A$12:A$200)-3),"")</f>
         <v/>
       </c>
-      <c r="B26" s="22">
+      <c r="C31" s="22">
         <f>IFERROR(INDEX(Registro!B$12:B$200,COUNTA(Registro!A$12:A$200)-3),"")</f>
         <v/>
       </c>
-      <c r="C26" s="22">
+      <c r="D31" s="22">
         <f>IFERROR(INDEX(Registro!C$12:C$200,COUNTA(Registro!A$12:A$200)-3),"")</f>
         <v/>
       </c>
-      <c r="D26" s="22">
+      <c r="E31" s="22">
         <f>IFERROR(INDEX(Registro!E$12:E$200,COUNTA(Registro!A$12:A$200)-3),"")</f>
         <v/>
       </c>
-      <c r="E26" s="22">
+      <c r="F31" s="22">
         <f>IFERROR(INDEX(Registro!F$12:F$200,COUNTA(Registro!A$12:A$200)-3),"")</f>
         <v/>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="19">
+    <row r="32">
+      <c r="B32" s="19">
         <f>IFERROR(INDEX(Registro!A$12:A$200,COUNTA(Registro!A$12:A$200)-4),"")</f>
         <v/>
       </c>
-      <c r="B27" s="20">
+      <c r="C32" s="20">
         <f>IFERROR(INDEX(Registro!B$12:B$200,COUNTA(Registro!A$12:A$200)-4),"")</f>
         <v/>
       </c>
-      <c r="C27" s="20">
+      <c r="D32" s="20">
         <f>IFERROR(INDEX(Registro!C$12:C$200,COUNTA(Registro!A$12:A$200)-4),"")</f>
         <v/>
       </c>
-      <c r="D27" s="20">
+      <c r="E32" s="20">
         <f>IFERROR(INDEX(Registro!E$12:E$200,COUNTA(Registro!A$12:A$200)-4),"")</f>
         <v/>
       </c>
-      <c r="E27" s="20">
+      <c r="F32" s="20">
         <f>IFERROR(INDEX(Registro!F$12:F$200,COUNTA(Registro!A$12:A$200)-4),"")</f>
         <v/>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="21">
+    <row r="33">
+      <c r="B33" s="21">
         <f>IFERROR(INDEX(Registro!A$12:A$200,COUNTA(Registro!A$12:A$200)-5),"")</f>
         <v/>
       </c>
-      <c r="B28" s="22">
+      <c r="C33" s="22">
         <f>IFERROR(INDEX(Registro!B$12:B$200,COUNTA(Registro!A$12:A$200)-5),"")</f>
         <v/>
       </c>
-      <c r="C28" s="22">
+      <c r="D33" s="22">
         <f>IFERROR(INDEX(Registro!C$12:C$200,COUNTA(Registro!A$12:A$200)-5),"")</f>
         <v/>
       </c>
-      <c r="D28" s="22">
+      <c r="E33" s="22">
         <f>IFERROR(INDEX(Registro!E$12:E$200,COUNTA(Registro!A$12:A$200)-5),"")</f>
         <v/>
       </c>
-      <c r="E28" s="22">
+      <c r="F33" s="22">
         <f>IFERROR(INDEX(Registro!F$12:F$200,COUNTA(Registro!A$12:A$200)-5),"")</f>
         <v/>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="19">
+    <row r="34">
+      <c r="B34" s="19">
         <f>IFERROR(INDEX(Registro!A$12:A$200,COUNTA(Registro!A$12:A$200)-6),"")</f>
         <v/>
       </c>
-      <c r="B29" s="20">
+      <c r="C34" s="20">
         <f>IFERROR(INDEX(Registro!B$12:B$200,COUNTA(Registro!A$12:A$200)-6),"")</f>
         <v/>
       </c>
-      <c r="C29" s="20">
+      <c r="D34" s="20">
         <f>IFERROR(INDEX(Registro!C$12:C$200,COUNTA(Registro!A$12:A$200)-6),"")</f>
         <v/>
       </c>
-      <c r="D29" s="20">
+      <c r="E34" s="20">
         <f>IFERROR(INDEX(Registro!E$12:E$200,COUNTA(Registro!A$12:A$200)-6),"")</f>
         <v/>
       </c>
-      <c r="E29" s="20">
+      <c r="F34" s="20">
         <f>IFERROR(INDEX(Registro!F$12:F$200,COUNTA(Registro!A$12:A$200)-6),"")</f>
         <v/>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="21">
+    <row r="35">
+      <c r="B35" s="21">
         <f>IFERROR(INDEX(Registro!A$12:A$200,COUNTA(Registro!A$12:A$200)-7),"")</f>
         <v/>
       </c>
-      <c r="B30" s="22">
+      <c r="C35" s="22">
         <f>IFERROR(INDEX(Registro!B$12:B$200,COUNTA(Registro!A$12:A$200)-7),"")</f>
         <v/>
       </c>
-      <c r="C30" s="22">
+      <c r="D35" s="22">
         <f>IFERROR(INDEX(Registro!C$12:C$200,COUNTA(Registro!A$12:A$200)-7),"")</f>
         <v/>
       </c>
-      <c r="D30" s="22">
+      <c r="E35" s="22">
         <f>IFERROR(INDEX(Registro!E$12:E$200,COUNTA(Registro!A$12:A$200)-7),"")</f>
         <v/>
       </c>
-      <c r="E30" s="22">
+      <c r="F35" s="22">
         <f>IFERROR(INDEX(Registro!F$12:F$200,COUNTA(Registro!A$12:A$200)-7),"")</f>
         <v/>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="19">
+    <row r="36">
+      <c r="B36" s="19">
         <f>IFERROR(INDEX(Registro!A$12:A$200,COUNTA(Registro!A$12:A$200)-8),"")</f>
         <v/>
       </c>
-      <c r="B31" s="20">
+      <c r="C36" s="20">
         <f>IFERROR(INDEX(Registro!B$12:B$200,COUNTA(Registro!A$12:A$200)-8),"")</f>
         <v/>
       </c>
-      <c r="C31" s="20">
+      <c r="D36" s="20">
         <f>IFERROR(INDEX(Registro!C$12:C$200,COUNTA(Registro!A$12:A$200)-8),"")</f>
         <v/>
       </c>
-      <c r="D31" s="20">
+      <c r="E36" s="20">
         <f>IFERROR(INDEX(Registro!E$12:E$200,COUNTA(Registro!A$12:A$200)-8),"")</f>
         <v/>
       </c>
-      <c r="E31" s="20">
+      <c r="F36" s="20">
         <f>IFERROR(INDEX(Registro!F$12:F$200,COUNTA(Registro!A$12:A$200)-8),"")</f>
         <v/>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="21">
+    <row r="37">
+      <c r="B37" s="21">
         <f>IFERROR(INDEX(Registro!A$12:A$200,COUNTA(Registro!A$12:A$200)-9),"")</f>
         <v/>
       </c>
-      <c r="B32" s="22">
+      <c r="C37" s="22">
         <f>IFERROR(INDEX(Registro!B$12:B$200,COUNTA(Registro!A$12:A$200)-9),"")</f>
         <v/>
       </c>
-      <c r="C32" s="22">
+      <c r="D37" s="22">
         <f>IFERROR(INDEX(Registro!C$12:C$200,COUNTA(Registro!A$12:A$200)-9),"")</f>
         <v/>
       </c>
-      <c r="D32" s="22">
+      <c r="E37" s="22">
         <f>IFERROR(INDEX(Registro!E$12:E$200,COUNTA(Registro!A$12:A$200)-9),"")</f>
         <v/>
       </c>
-      <c r="E32" s="22">
+      <c r="F37" s="22">
         <f>IFERROR(INDEX(Registro!F$12:F$200,COUNTA(Registro!A$12:A$200)-9),"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A2:E2"/>
+  <mergeCells count="22">
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="H6:I7"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="J6:K7"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B26:F26"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4168,7 +4773,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4351,7 +4956,7 @@
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>HOJA 'PROGRESO'</t>
+          <t>HOJA 'DASHBOARD'</t>
         </is>
       </c>
       <c r="B19" s="6" t="n"/>
@@ -4364,7 +4969,7 @@
       </c>
       <c r="B20" s="26" t="inlineStr">
         <is>
-          <t>Muestra estadísticas automáticas calculadas desde tu historial.</t>
+          <t>Dashboard visual con KPIs, gráficos e insights de tu progreso.</t>
         </is>
       </c>
     </row>
@@ -4376,7 +4981,7 @@
       </c>
       <c r="B21" s="26" t="inlineStr">
         <is>
-          <t>Total de sesiones, peso máximo, promedios y volumen por día.</t>
+          <t>5 tarjetas de métricas clave: sesiones, último entreno, peso máx, etc.</t>
         </is>
       </c>
     </row>
@@ -4388,17 +4993,33 @@
       </c>
       <c r="B22" s="26" t="inlineStr">
         <is>
-          <t>Los últimos 10 registros se muestran al final.</t>
+          <t>Gráfico de barras: sesiones por día de rutina.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="20" t="inlineStr">
+        <is>
+          <t>•</t>
+        </is>
+      </c>
+      <c r="B23" s="26" t="inlineStr">
+        <is>
+          <t>Gráfico circular: distribución porcentual de entrenamientos.</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="5" t="inlineStr">
-        <is>
-          <t>TIPS</t>
-        </is>
-      </c>
-      <c r="B24" s="6" t="n"/>
+      <c r="A24" s="20" t="inlineStr">
+        <is>
+          <t>•</t>
+        </is>
+      </c>
+      <c r="B24" s="26" t="inlineStr">
+        <is>
+          <t>Gráfico de línea: progresión del peso levantado por sesión.</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="20" t="inlineStr">
@@ -4408,7 +5029,7 @@
       </c>
       <c r="B25" s="26" t="inlineStr">
         <is>
-          <t>Registra CADA serie por separado para un seguimiento más detallado.</t>
+          <t>Sección de insights: días sin entrenar, sesiones semanales/mensuales.</t>
         </is>
       </c>
     </row>
@@ -4420,29 +5041,61 @@
       </c>
       <c r="B26" s="26" t="inlineStr">
         <is>
+          <t>Los últimos 10 registros se muestran al final.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5" t="inlineStr">
+        <is>
+          <t>TIPS</t>
+        </is>
+      </c>
+      <c r="B28" s="6" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="20" t="inlineStr">
+        <is>
+          <t>•</t>
+        </is>
+      </c>
+      <c r="B29" s="26" t="inlineStr">
+        <is>
+          <t>Registra CADA serie por separado para un seguimiento más detallado.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="20" t="inlineStr">
+        <is>
+          <t>•</t>
+        </is>
+      </c>
+      <c r="B30" s="26" t="inlineStr">
+        <is>
           <t>O registra el total de series/reps por ejercicio si prefieres algo rápido.</t>
         </is>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="20" t="inlineStr">
+    <row r="31">
+      <c r="A31" s="20" t="inlineStr">
         <is>
           <t>•</t>
         </is>
       </c>
-      <c r="B27" s="26" t="inlineStr">
+      <c r="B31" s="26" t="inlineStr">
         <is>
           <t>Revisa la hoja de Progreso regularmente para ver tu avance.</t>
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="20" t="inlineStr">
+    <row r="32">
+      <c r="A32" s="20" t="inlineStr">
         <is>
           <t>•</t>
         </is>
       </c>
-      <c r="B28" s="26" t="inlineStr">
+      <c r="B32" s="26" t="inlineStr">
         <is>
           <t>¡La constancia es la clave! Intenta entrenar al menos 3-4 días por semana.</t>
         </is>
@@ -4450,8 +5103,8 @@
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:B3"/>

</xml_diff>